<commit_message>
Update NCTU DS HW2 20210613
</commit_message>
<xml_diff>
--- a/Data Structures and Object-oriented Programming/NCTU/HW2/execution.xlsx
+++ b/Data Structures and Object-oriented Programming/NCTU/HW2/execution.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94215301-00C6-0F4A-AB92-D61A4F63C9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41212EEC-2670-DD4A-B610-222739D2BDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="1620" windowWidth="25960" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="1360" windowWidth="29840" windowHeight="20300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>qsort</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,13 +82,25 @@
     <t>n = 128000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quick sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -127,7 +140,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -143,6 +156,1268 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>Execution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+              <a:t> time comparision</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15302312646466815"/>
+          <c:y val="0.14260233712114456"/>
+          <c:w val="0.79752119096278407"/>
+          <c:h val="0.66281804619338569"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>13.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>214.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>454.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>948.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2021.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E5D8-8F44-A2A7-F38A7DB2F814}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>18.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>153.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>316.83999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>669.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1419.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3057.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E5D8-8F44-A2A7-F38A7DB2F814}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1020952976"/>
+        <c:axId val="1020972736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1020952976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="13000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+                  <a:t>Input</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1200" baseline="0"/>
+                  <a:t> array size (#)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1020972736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1020972736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1200"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1200" baseline="0"/>
+                  <a:t> time (µs)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1020952976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26385683053805742"/>
+          <c:y val="0.23702563313963054"/>
+          <c:w val="0.19805637918423472"/>
+          <c:h val="0.15225404929582612"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>143934</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>33866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>668866</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFE3BCE7-C9CD-1E43-BC9B-E2FC24DE8E30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A92" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -5626,4 +6901,154 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F110779B-E208-674B-9839-1572B6EABEF0}">
+  <dimension ref="A1:S9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>13.57</v>
+      </c>
+      <c r="C2">
+        <v>18.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3">
+        <f xml:space="preserve"> 2*A2</f>
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>28.36</v>
+      </c>
+      <c r="C3">
+        <v>40.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4">
+        <f xml:space="preserve"> 2 * A3</f>
+        <v>400</v>
+      </c>
+      <c r="B4">
+        <v>60.87</v>
+      </c>
+      <c r="C4">
+        <v>86.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5">
+        <f xml:space="preserve"> 2*A4</f>
+        <v>800</v>
+      </c>
+      <c r="B5">
+        <v>105.7</v>
+      </c>
+      <c r="C5">
+        <v>153.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6">
+        <f xml:space="preserve"> 2*A5</f>
+        <v>1600</v>
+      </c>
+      <c r="B6">
+        <v>214.05</v>
+      </c>
+      <c r="C6">
+        <v>316.83999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7">
+        <f xml:space="preserve"> 2 * A6</f>
+        <v>3200</v>
+      </c>
+      <c r="B7">
+        <v>454.66</v>
+      </c>
+      <c r="C7">
+        <v>669.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8">
+        <f xml:space="preserve"> 2*A7</f>
+        <v>6400</v>
+      </c>
+      <c r="B8">
+        <v>948.42</v>
+      </c>
+      <c r="C8">
+        <v>1419.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9">
+        <f xml:space="preserve"> 2*A8</f>
+        <v>12800</v>
+      </c>
+      <c r="B9">
+        <v>2021.42</v>
+      </c>
+      <c r="C9">
+        <v>3057.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A7 A4" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>